<commit_message>
new report for comisiones
</commit_message>
<xml_diff>
--- a/public/Reportes/reservaciones/reservaciones.xlsx
+++ b/public/Reportes/reservaciones/reservaciones.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Delfiniti de México S.A. de C.V.</t>
   </si>
@@ -23,7 +23,7 @@
     <t>REPORTE DE RESERVACIONES</t>
   </si>
   <si>
-    <t>Del 15-08-2022 al 15-08-2022</t>
+    <t>Del 17-08-2022 al 17-08-2022</t>
   </si>
   <si>
     <t>FAMILY CLUB MED 10:00:00</t>
@@ -44,25 +44,16 @@
     <t>T. PAGO</t>
   </si>
   <si>
-    <t>JORGE IVAN GOMEZ</t>
+    <t>JORGE</t>
   </si>
   <si>
     <t>efectivo</t>
   </si>
   <si>
-    <t>FAMILY CLUB MED 10:30:00</t>
-  </si>
-  <si>
-    <t>JROGE IVAN GOMEZ CARRANZA</t>
-  </si>
-  <si>
-    <t>FAMILY CLUB MED 12:00:00</t>
-  </si>
-  <si>
-    <t>JROGEIV</t>
-  </si>
-  <si>
-    <t>NURIA ZENDEJAS</t>
+    <t>ENCUENTRO 10:00:00</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
   <si>
     <t>PROGRAMA</t>
@@ -71,6 +62,9 @@
     <t>PAGADOS</t>
   </si>
   <si>
+    <t>PENDIENTES</t>
+  </si>
+  <si>
     <t>CORTESIAS</t>
   </si>
   <si>
@@ -78,6 +72,9 @@
   </si>
   <si>
     <t>FAMILY CLUB MED</t>
+  </si>
+  <si>
+    <t>ENCUENTRO</t>
   </si>
 </sst>
 </file>
@@ -509,10 +506,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A33" sqref="A33:D33"/>
+      <selection activeCell="A21" sqref="A21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.83203125" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -521,7 +518,7 @@
     <col min="2" max="2" width="14.83203125" customWidth="true" style="1"/>
     <col min="3" max="3" width="12.5" customWidth="true" style="1"/>
     <col min="4" max="4" width="9.1640625" customWidth="true" style="1"/>
-    <col min="5" max="5" width="9.1640625" customWidth="true" style="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="true" style="1"/>
     <col min="6" max="6" width="11.83203125" customWidth="true" style="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="true" style="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="true" style="1"/>
@@ -634,256 +631,124 @@
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12">
+      <c r="D8" s="1">
+        <f>SUM(D7:D7)</f>
         <v>1</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12">
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12">
+        <v>5</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="D13" s="1">
+        <f>SUM(D12:D12)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUM(B19:D19)</f>
         <v>1</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12">
-        <v>1</v>
-      </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="D12" s="1">
-        <f>SUM(D7:D11)</f>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11" t="s">
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUM(B20:D20)</f>
         <v>5</v>
       </c>
-      <c r="D15" s="11" t="s">
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10">
+        <f>SUM(B19:B20)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="10">
+        <f>SUM(C19:C20)</f>
         <v>6</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12">
-        <v>1</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12">
-        <v>1</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12">
-        <v>1</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="D21" s="1">
-        <f>SUM(D16:D20)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="D21" s="10">
+        <f>SUM(D19:D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f>SUM(E19:E20)</f>
         <v>6</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12">
-        <v>1</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="D26" s="1">
-        <f>SUM(D25:D25)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="1">
-        <v>10</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0</v>
-      </c>
-      <c r="D32" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10">
-        <f>SUM(B32:B32)</f>
-        <v>10</v>
-      </c>
-      <c r="C33" s="10">
-        <f>SUM(C32:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="10">
-        <f>SUM(D32:D32)</f>
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -895,20 +760,9 @@
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "new tipo pago"
This reverts commit d50364e2a2acb8c5b08838bcc6360fff9f82f5eb.
</commit_message>
<xml_diff>
--- a/public/Reportes/reservaciones/reservaciones.xlsx
+++ b/public/Reportes/reservaciones/reservaciones.xlsx
@@ -15,15 +15,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
-  <si>
-    <t>DELFINITI DE MÉXICO S.A DE C.V</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>Delfiniti de México S.A. de C.V.</t>
   </si>
   <si>
     <t>REPORTE DE RESERVACIONES</t>
   </si>
   <si>
-    <t>Del 06-10-2022 al 06-10-2022</t>
+    <t>Del 17-08-2022 al 17-08-2022</t>
+  </si>
+  <si>
+    <t>FAMILY CLUB MED 10:00:00</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>ORIGEN</t>
+  </si>
+  <si>
+    <t>PAX</t>
+  </si>
+  <si>
+    <t>AGENTE/AGENCIA</t>
+  </si>
+  <si>
+    <t>T. PAGO</t>
+  </si>
+  <si>
+    <t>JORGE</t>
+  </si>
+  <si>
+    <t>efectivo</t>
+  </si>
+  <si>
+    <t>ENCUENTRO 10:00:00</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
   <si>
     <t>PROGRAMA</t>
@@ -39,6 +69,12 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>FAMILY CLUB MED</t>
+  </si>
+  <si>
+    <t>ENCUENTRO</t>
   </si>
 </sst>
 </file>
@@ -46,7 +82,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -83,53 +119,8 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="26"/>
-      <color rgb="FF17365D"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="12"/>
-      <color rgb="FF17365D"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="20"/>
-      <color rgb="FF17365D"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,23 +129,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FF17365D"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFABF8F"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F000"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -176,19 +186,25 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="5" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="6" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="7" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="3" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="8" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="4" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="5" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="6" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -490,21 +506,21 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A9" sqref="A9:E9"/>
+      <selection activeCell="A21" sqref="A21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.83203125" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="true" customWidth="true" style="1"/>
-    <col min="2" max="2" width="9" bestFit="true" customWidth="true" style="1"/>
-    <col min="3" max="3" width="13" bestFit="true" customWidth="true" style="1"/>
-    <col min="4" max="4" width="12" bestFit="true" customWidth="true" style="1"/>
-    <col min="5" max="5" width="7" bestFit="true" customWidth="true" style="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="true" style="1"/>
-    <col min="7" max="7" width="8.83203125" bestFit="true" style="1"/>
+    <col min="1" max="1" width="14.5" customWidth="true" style="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="true" style="1"/>
+    <col min="3" max="3" width="12.5" customWidth="true" style="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="true" style="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="true" style="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="true" style="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="true" style="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="true" style="1"/>
   </cols>
   <sheetData>
@@ -575,40 +591,164 @@
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
     </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="10" t="s">
+      <c r="D8" s="1">
+        <f>SUM(D7:D7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11">
-        <f>SUM(B9:B8)</f>
+      <c r="F11" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12">
+        <v>5</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="D13" s="1">
+        <f>SUM(D12:D12)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
         <v>0</v>
       </c>
-      <c r="C9" s="11">
-        <f>SUM(C9:C8)</f>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="D9" s="11">
-        <f>SUM(D9:D8)</f>
+      <c r="E19" s="1">
+        <f>SUM(B19:D19)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="11">
-        <f>SUM(E9:E8)</f>
+      <c r="C20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
         <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUM(B20:D20)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10">
+        <f>SUM(B19:B20)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="10">
+        <f>SUM(C19:C20)</f>
+        <v>6</v>
+      </c>
+      <c r="D21" s="10">
+        <f>SUM(D19:D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f>SUM(E19:E20)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -617,6 +757,12 @@
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>